<commit_message>
userInterface to run the bot
</commit_message>
<xml_diff>
--- a/dataSource/SI_Satisfaction_RegData.xlsx
+++ b/dataSource/SI_Satisfaction_RegData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Veritas\SatfnReg.InvBot\dataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308EA83C-163E-4157-8E8E-FDB0A4899E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733F0C4E-8F9D-4D35-94E1-FC75F183FFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F9B19C6-B628-4404-9EC4-73CCC5C2890C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$281</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,15 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Closed Date</t>
   </si>
   <si>
     <t>CERSAI Regist No</t>
-  </si>
-  <si>
-    <t>Trans ID</t>
   </si>
 </sst>
 </file>
@@ -115,13 +112,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8784E028-444E-42E3-82C6-19C6FD56C5B1}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -446,22 +442,18 @@
   <cols>
     <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C281" xr:uid="{8784E028-444E-42E3-82C6-19C6FD56C5B1}"/>
+  <autoFilter ref="A1:B281" xr:uid="{8784E028-444E-42E3-82C6-19C6FD56C5B1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>